<commit_message>
Fix ai response and add requirements for python venv
</commit_message>
<xml_diff>
--- a/translation.xlsx
+++ b/translation.xlsx
@@ -1006,7 +1006,7 @@
     <t xml:space="preserve">wait_ai_response</t>
   </si>
   <si>
-    <t xml:space="preserve">Ожидайте ответа</t>
+    <t xml:space="preserve">Ожидайте ответ</t>
   </si>
   <si>
     <t xml:space="preserve">Expect a response</t>
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B26" activeCellId="0" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>